<commit_message>
Updates to use Excel plugin dll from bin\release of source project
</commit_message>
<xml_diff>
--- a/Itamaram.Excel.SpecFlowPlugin.DotNetCore.IntegrationTests/Features/Book1.xlsx
+++ b/Itamaram.Excel.SpecFlowPlugin.DotNetCore.IntegrationTests/Features/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\SpecFlow.Plugin.Base\Itamaram.Excel.SpecFlowPlugin.DotNetCore.IntegrationTests\Features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kreddyva\Source\Repos\rkkreddy\SpecFlow.Plugin.Base\Itamaram.Excel.SpecFlowPlugin.DotNetCore.IntegrationTests\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A254FD03-A46F-40DE-885E-94A1A1A6DB8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1928D86A-F7C2-4B2B-90A1-EDA7DFAE729A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{48E912E3-F508-4588-AE82-830AA8426E11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48E912E3-F508-4588-AE82-830AA8426E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,11 +26,30 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>great</t>
+  </si>
+  <si>
+    <t>teest</t>
+  </si>
+  <si>
+    <t>Threee</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,23 +399,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645C1B7A-D566-422F-AC14-AD15B2F1B8C4}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1">
-        <v>10</v>
-      </c>
-      <c r="B1">
-        <v>20</v>
-      </c>
-      <c r="C1">
-        <v>30</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>121</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>112</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to read SkipFirstRow from ItamaramExcelConfig.json and skip and read first row of excel as column headers
</commit_message>
<xml_diff>
--- a/Itamaram.Excel.SpecFlowPlugin.DotNetCore.IntegrationTests/Features/Book1.xlsx
+++ b/Itamaram.Excel.SpecFlowPlugin.DotNetCore.IntegrationTests/Features/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kreddyva\Source\Repos\rkkreddy\SpecFlow.Plugin.Base\Itamaram.Excel.SpecFlowPlugin.DotNetCore.IntegrationTests\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1928D86A-F7C2-4B2B-90A1-EDA7DFAE729A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3800C73-F5BB-45B5-88F4-212A045491CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48E912E3-F508-4588-AE82-830AA8426E11}"/>
   </bookViews>
@@ -41,13 +41,13 @@
     <t>Two</t>
   </si>
   <si>
-    <t>great</t>
+    <t>Three</t>
   </si>
   <si>
-    <t>teest</t>
+    <t>Four</t>
   </si>
   <si>
-    <t>Threee</t>
+    <t>Five</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,13 +415,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>